<commit_message>
all entropy calculations have been performed
</commit_message>
<xml_diff>
--- a/code/results/entropy_C_sampen_4_1_0.8_inicial_stats.xlsx
+++ b/code/results/entropy_C_sampen_4_1_0.8_inicial_stats.xlsx
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>4.482395957300334e-39</v>
+        <v>4.482395957300335e-39</v>
       </c>
       <c r="F11" t="n">
         <v>12.51952247963914</v>
@@ -968,7 +968,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>3.789909202236127e-15</v>
+        <v>3.789909202236128e-15</v>
       </c>
       <c r="F18" t="n">
         <v>-12.07406915840211</v>
@@ -1088,7 +1088,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.05882032335312916</v>
+        <v>0.05882032335312914</v>
       </c>
       <c r="F22" t="n">
         <v>1.182156656690444</v>

</xml_diff>